<commit_message>
implement worksheet_formula for xlsx
</commit_message>
<xml_diff>
--- a/tests/issues.xlsx
+++ b/tests/issues.xlsx
@@ -504,12 +504,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <f>B1+OneRange</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>